<commit_message>
refactor code, auto load data after add or delete
</commit_message>
<xml_diff>
--- a/excel/subject 15.14.38.xlsx
+++ b/excel/subject 15.14.38.xlsx
@@ -14,13 +14,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
-    <t>Mã môn</t>
-  </si>
-  <si>
-    <t>Tên môn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Số tín chỉ </t>
+    <t>code_subject</t>
+  </si>
+  <si>
+    <t>name_subject</t>
+  </si>
+  <si>
+    <t>credit</t>
   </si>
   <si>
     <t>INT2001</t>
@@ -1363,7 +1363,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" ht="14.7" customHeight="1">

</xml_diff>